<commit_message>
added save to my charts
</commit_message>
<xml_diff>
--- a/SaaS.xlsx
+++ b/SaaS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vasiliki\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SaaS2023\SaaS23-42\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6379CBD-02EC-473D-917D-591C437774C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361480BF-8CBA-497D-81BB-780EE020EBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>1.</t>
   </si>
@@ -90,9 +90,6 @@
     <t>createDiagram</t>
   </si>
   <si>
-    <t>deleteDiagram</t>
-  </si>
-  <si>
     <t>convertDiagram</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>6. CONVERT TO X MICROSERVICE</t>
   </si>
   <si>
-    <t>7.</t>
-  </si>
-  <si>
     <t>1.verifyLogin, 2.createUser, 3.createUser</t>
   </si>
   <si>
@@ -148,12 +142,6 @@
   </si>
   <si>
     <t>1.isLoggedIn, 2.subQuotas, 3.saveChart</t>
-  </si>
-  <si>
-    <t>discardChart</t>
-  </si>
-  <si>
-    <t>1.isLoggedIn, 5.deleteDiagram</t>
   </si>
   <si>
     <t>8.</t>
@@ -261,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -276,6 +264,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +563,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -597,7 +588,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -758,7 +749,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -879,7 +870,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -920,7 +911,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1058,7 +1049,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1144,7 +1135,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1189,12 +1180,8 @@
       <c r="R27" s="2"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1234,7 +1221,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1259,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1300,7 +1287,7 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1328,10 +1315,10 @@
         <v>8</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -1356,10 +1343,10 @@
         <v>9</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -1381,13 +1368,13 @@
         <v>3</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1412,10 +1399,10 @@
         <v>19</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -1426,13 +1413,13 @@
         <v>5</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E38" s="2"/>
     </row>
@@ -1441,89 +1428,81 @@
         <v>6</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>